<commit_message>
added stats comparisons and plots for failure loads
</commit_message>
<xml_diff>
--- a/CouponData/CouponIDDataSheetReformat.xlsx
+++ b/CouponData/CouponIDDataSheetReformat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\SurfboardProj\SurfURS\CouponData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C454ADF3-3EFE-4714-ABA6-80DDC8343ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD51D6B4-5D4C-4731-964B-8FEECB51A4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>China Balsa Blue on Bottom</t>
+  </si>
+  <si>
+    <t>China Balsa Blue on Top Foam Shear Fail</t>
   </si>
 </sst>
 </file>
@@ -514,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +941,7 @@
         <v>11</v>
       </c>
       <c r="O9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding testing data from day 3
</commit_message>
<xml_diff>
--- a/CouponData/CouponIDDataSheetReformat.xlsx
+++ b/CouponData/CouponIDDataSheetReformat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\SurfboardProj\SurfURS\CouponData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\SurfboardProj\SurfURS\CouponData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD51D6B4-5D4C-4731-964B-8FEECB51A4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED509A45-ABD4-4DE6-B1AE-A8F476401927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Eglass4oz</t>
   </si>
   <si>
-    <t>Birchwood</t>
-  </si>
-  <si>
     <t>Eglass4oz,Eglass6oz</t>
   </si>
   <si>
@@ -167,18 +164,6 @@
     <t>ID120</t>
   </si>
   <si>
-    <t>ID201</t>
-  </si>
-  <si>
-    <t>ID202</t>
-  </si>
-  <si>
-    <t>ID203</t>
-  </si>
-  <si>
-    <t>ID204</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -198,6 +183,87 @@
   </si>
   <si>
     <t>China Balsa Blue on Top Foam Shear Fail</t>
+  </si>
+  <si>
+    <t>ID301</t>
+  </si>
+  <si>
+    <t>ID302</t>
+  </si>
+  <si>
+    <t>ID303</t>
+  </si>
+  <si>
+    <t>ID304</t>
+  </si>
+  <si>
+    <t>ID305</t>
+  </si>
+  <si>
+    <t>ID401</t>
+  </si>
+  <si>
+    <t>ID402</t>
+  </si>
+  <si>
+    <t>ID403</t>
+  </si>
+  <si>
+    <t>ID404</t>
+  </si>
+  <si>
+    <t>ID501</t>
+  </si>
+  <si>
+    <t>ID601</t>
+  </si>
+  <si>
+    <t>1ply carbon</t>
+  </si>
+  <si>
+    <t>Strong on Top</t>
+  </si>
+  <si>
+    <t>1ply carbon sheet shear</t>
+  </si>
+  <si>
+    <t>surface aluminum sheet shear</t>
+  </si>
+  <si>
+    <t>Uni Carbon buckle</t>
+  </si>
+  <si>
+    <t>Balsa Skin sheet shear</t>
+  </si>
+  <si>
+    <t>ID401B</t>
+  </si>
+  <si>
+    <t>ID404B</t>
+  </si>
+  <si>
+    <t>ID801</t>
+  </si>
+  <si>
+    <t>ID802</t>
+  </si>
+  <si>
+    <t>ID1001</t>
+  </si>
+  <si>
+    <t>ID1002</t>
+  </si>
+  <si>
+    <t>OverVacuumed No Balsa</t>
+  </si>
+  <si>
+    <t>Expanded Foam Honeycomb</t>
+  </si>
+  <si>
+    <t>ID1101</t>
+  </si>
+  <si>
+    <t>Carbon Balsa Wood</t>
   </si>
 </sst>
 </file>
@@ -515,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,22 +632,22 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
       <c r="L1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
       <c r="O1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -592,10 +658,10 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -628,10 +694,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -658,16 +724,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -676,7 +742,7 @@
         <v>0.125</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G27" si="0">0.00025*1/(0.0254)</f>
+        <f t="shared" ref="G4:G41" si="0">0.00025*1/(0.0254)</f>
         <v>9.8425196850393699E-3</v>
       </c>
       <c r="H4">
@@ -692,7 +758,7 @@
         <v>310.8</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>4</v>
@@ -701,21 +767,21 @@
         <v>11</v>
       </c>
       <c r="O4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -740,7 +806,7 @@
         <v>327.3</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M5">
         <v>4</v>
@@ -749,21 +815,21 @@
         <v>11</v>
       </c>
       <c r="O5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -788,7 +854,7 @@
         <v>289.39999999999998</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -797,21 +863,21 @@
         <v>11</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -836,7 +902,7 @@
         <v>325.7</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M7">
         <v>4</v>
@@ -845,21 +911,21 @@
         <v>11</v>
       </c>
       <c r="O7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -884,7 +950,7 @@
         <v>244.1</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M8">
         <v>4</v>
@@ -893,21 +959,21 @@
         <v>11</v>
       </c>
       <c r="O8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -932,7 +998,7 @@
         <v>267.2</v>
       </c>
       <c r="L9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M9">
         <v>4</v>
@@ -941,21 +1007,21 @@
         <v>11</v>
       </c>
       <c r="O9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -980,7 +1046,7 @@
         <v>285.89999999999998</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M10">
         <v>4</v>
@@ -989,21 +1055,21 @@
         <v>11</v>
       </c>
       <c r="O10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1028,7 +1094,7 @@
         <v>278.7</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11">
         <v>4</v>
@@ -1037,21 +1103,21 @@
         <v>11</v>
       </c>
       <c r="O11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1076,7 +1142,7 @@
         <v>288.39999999999998</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <v>4</v>
@@ -1085,21 +1151,21 @@
         <v>11</v>
       </c>
       <c r="O12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1124,7 +1190,7 @@
         <v>266.60000000000002</v>
       </c>
       <c r="L13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M13">
         <v>4</v>
@@ -1133,21 +1199,21 @@
         <v>11</v>
       </c>
       <c r="O13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1172,7 +1238,7 @@
         <v>239.5</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M14">
         <v>4</v>
@@ -1181,21 +1247,21 @@
         <v>11</v>
       </c>
       <c r="O14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1220,7 +1286,7 @@
         <v>265.7</v>
       </c>
       <c r="L15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M15">
         <v>4</v>
@@ -1229,21 +1295,21 @@
         <v>11</v>
       </c>
       <c r="O15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1268,7 +1334,7 @@
         <v>307.8</v>
       </c>
       <c r="L16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M16">
         <v>4</v>
@@ -1277,21 +1343,21 @@
         <v>11</v>
       </c>
       <c r="O16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1316,7 +1382,7 @@
         <v>308.7</v>
       </c>
       <c r="L17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M17">
         <v>4</v>
@@ -1325,21 +1391,21 @@
         <v>11</v>
       </c>
       <c r="O17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1364,7 +1430,7 @@
         <v>279</v>
       </c>
       <c r="L18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M18">
         <v>4</v>
@@ -1373,21 +1439,21 @@
         <v>11</v>
       </c>
       <c r="O18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1412,7 +1478,7 @@
         <v>264.7</v>
       </c>
       <c r="L19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19">
         <v>4</v>
@@ -1421,21 +1487,21 @@
         <v>11</v>
       </c>
       <c r="O19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1460,7 +1526,7 @@
         <v>262.7</v>
       </c>
       <c r="L20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M20">
         <v>4</v>
@@ -1469,21 +1535,21 @@
         <v>11</v>
       </c>
       <c r="O20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -1508,7 +1574,7 @@
         <v>278.5</v>
       </c>
       <c r="L21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M21">
         <v>4</v>
@@ -1517,21 +1583,21 @@
         <v>11</v>
       </c>
       <c r="O21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1556,7 +1622,7 @@
         <v>291.7</v>
       </c>
       <c r="L22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M22">
         <v>4</v>
@@ -1565,21 +1631,21 @@
         <v>11</v>
       </c>
       <c r="O22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1604,7 +1670,7 @@
         <v>284.7</v>
       </c>
       <c r="L23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M23">
         <v>4</v>
@@ -1613,27 +1679,27 @@
         <v>11</v>
       </c>
       <c r="O23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24">
-        <v>0.125</v>
+        <v>1.125</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
@@ -1644,26 +1710,44 @@
       </c>
       <c r="I24">
         <v>2.5</v>
+      </c>
+      <c r="J24">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K24">
+        <v>249.8</v>
+      </c>
+      <c r="L24" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>11</v>
+      </c>
+      <c r="O24" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
       </c>
       <c r="F25">
-        <v>0.125</v>
+        <v>2.125</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
@@ -1674,26 +1758,44 @@
       </c>
       <c r="I25">
         <v>2.5</v>
+      </c>
+      <c r="J25">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K25">
+        <v>243.4</v>
+      </c>
+      <c r="L25" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25">
+        <v>4</v>
+      </c>
+      <c r="N25">
+        <v>11</v>
+      </c>
+      <c r="O25" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
       </c>
       <c r="F26">
-        <v>0.125</v>
+        <v>3.125</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -1704,26 +1806,44 @@
       </c>
       <c r="I26">
         <v>2.5</v>
+      </c>
+      <c r="J26">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K26">
+        <v>250.4</v>
+      </c>
+      <c r="L26" t="s">
+        <v>61</v>
+      </c>
+      <c r="M26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <v>11</v>
+      </c>
+      <c r="O26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27">
-        <v>0.125</v>
+        <v>4.125</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
@@ -1734,6 +1854,696 @@
       </c>
       <c r="I27">
         <v>2.5</v>
+      </c>
+      <c r="J27">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K27">
+        <v>252.3</v>
+      </c>
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>11</v>
+      </c>
+      <c r="O27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>5.125</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H28">
+        <v>6</v>
+      </c>
+      <c r="I28">
+        <v>2.5</v>
+      </c>
+      <c r="J28">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K28">
+        <v>251</v>
+      </c>
+      <c r="L28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M28">
+        <v>4</v>
+      </c>
+      <c r="N28">
+        <v>11</v>
+      </c>
+      <c r="O28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>6.125</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="I29">
+        <v>2.5</v>
+      </c>
+      <c r="J29">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K29">
+        <v>256.2</v>
+      </c>
+      <c r="L29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <v>11</v>
+      </c>
+      <c r="O29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30">
+        <v>7.125</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="I30">
+        <v>2.5</v>
+      </c>
+      <c r="J30">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K30">
+        <v>256.2</v>
+      </c>
+      <c r="L30" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30">
+        <v>11</v>
+      </c>
+      <c r="O30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31">
+        <v>7.125</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <v>2.5</v>
+      </c>
+      <c r="J31">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K31">
+        <v>236.2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31">
+        <v>4</v>
+      </c>
+      <c r="N31">
+        <v>11</v>
+      </c>
+      <c r="O31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>8.125</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32">
+        <v>2.5</v>
+      </c>
+      <c r="J32">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K32">
+        <v>251.3</v>
+      </c>
+      <c r="L32" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32">
+        <v>4</v>
+      </c>
+      <c r="N32">
+        <v>11</v>
+      </c>
+      <c r="O32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>9.125</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H33">
+        <v>6</v>
+      </c>
+      <c r="I33">
+        <v>2.5</v>
+      </c>
+      <c r="J33">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K33">
+        <v>275.8</v>
+      </c>
+      <c r="L33" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33">
+        <v>4</v>
+      </c>
+      <c r="N33">
+        <v>11</v>
+      </c>
+      <c r="O33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <v>10.125</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H34">
+        <v>6</v>
+      </c>
+      <c r="I34">
+        <v>2.5</v>
+      </c>
+      <c r="J34">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K34">
+        <v>275.8</v>
+      </c>
+      <c r="L34" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34">
+        <v>4</v>
+      </c>
+      <c r="N34">
+        <v>11</v>
+      </c>
+      <c r="O34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>10.125</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H35">
+        <v>6</v>
+      </c>
+      <c r="I35">
+        <v>2.5</v>
+      </c>
+      <c r="J35">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K35">
+        <v>227.7</v>
+      </c>
+      <c r="L35" t="s">
+        <v>61</v>
+      </c>
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>11</v>
+      </c>
+      <c r="O35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <v>11.125</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>2.5</v>
+      </c>
+      <c r="J36">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K36">
+        <v>279.7</v>
+      </c>
+      <c r="L36" t="s">
+        <v>61</v>
+      </c>
+      <c r="M36">
+        <v>4</v>
+      </c>
+      <c r="N36">
+        <v>11</v>
+      </c>
+      <c r="O36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <v>12.125</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H37">
+        <v>6</v>
+      </c>
+      <c r="I37">
+        <v>2.5</v>
+      </c>
+      <c r="J37">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K37">
+        <v>279.7</v>
+      </c>
+      <c r="L37" t="s">
+        <v>61</v>
+      </c>
+      <c r="M37">
+        <v>4</v>
+      </c>
+      <c r="N37">
+        <v>11</v>
+      </c>
+      <c r="O37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>13.125</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38">
+        <v>2.5</v>
+      </c>
+      <c r="J38">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K38">
+        <v>279.7</v>
+      </c>
+      <c r="L38" t="s">
+        <v>61</v>
+      </c>
+      <c r="M38">
+        <v>4</v>
+      </c>
+      <c r="N38">
+        <v>11</v>
+      </c>
+      <c r="O38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>14.125</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H39">
+        <v>6</v>
+      </c>
+      <c r="I39">
+        <v>2.5</v>
+      </c>
+      <c r="J39">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K39">
+        <v>279.7</v>
+      </c>
+      <c r="L39" t="s">
+        <v>61</v>
+      </c>
+      <c r="M39">
+        <v>4</v>
+      </c>
+      <c r="N39">
+        <v>11</v>
+      </c>
+      <c r="O39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40">
+        <v>15.125</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40">
+        <v>2.5</v>
+      </c>
+      <c r="J40">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K40">
+        <v>279.7</v>
+      </c>
+      <c r="L40" t="s">
+        <v>61</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>11</v>
+      </c>
+      <c r="O40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41">
+        <v>16.125</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>9.8425196850393699E-3</v>
+      </c>
+      <c r="H41">
+        <v>6</v>
+      </c>
+      <c r="I41">
+        <v>2.5</v>
+      </c>
+      <c r="J41">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="K41">
+        <v>279.7</v>
+      </c>
+      <c r="L41" t="s">
+        <v>61</v>
+      </c>
+      <c r="M41">
+        <v>4</v>
+      </c>
+      <c r="N41">
+        <v>11</v>
+      </c>
+      <c r="O41" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>